<commit_message>
Logboek en C# design.
</commit_message>
<xml_diff>
--- a/Algemeen/Logboek/Logboek Roel Kusters.xlsx
+++ b/Algemeen/Logboek/Logboek Roel Kusters.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjmku\Documents\School\Jaar2\S4\3_DI_Proftaak\Git\PTT41\Algemeen\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC5269E-55F9-4A9F-8461-D4C6334E151C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C47002-DCBA-44DD-B766-7BD718247DCC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{1FDE790C-1098-453A-B25A-4B8D392970A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="57">
   <si>
     <t>Tijd geëindigd</t>
   </si>
@@ -137,9 +138,6 @@
     <t>Vergadering netwerk met ander team</t>
   </si>
   <si>
-    <t>Afstemming netwerk gedeelte van proftaak met het andere team.</t>
-  </si>
-  <si>
     <t>Oplossen router</t>
   </si>
   <si>
@@ -164,10 +162,46 @@
     <t>Begin van design van com classen diagram</t>
   </si>
   <si>
-    <t>documentatie</t>
-  </si>
-  <si>
     <t>Week 7</t>
+  </si>
+  <si>
+    <t>Bouwen test plc</t>
+  </si>
+  <si>
+    <t>Opzetten software test plc</t>
+  </si>
+  <si>
+    <t>Overleg met klant</t>
+  </si>
+  <si>
+    <t>Opzetten router networking</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Onderzoek MQTT server libraries</t>
+  </si>
+  <si>
+    <t>Onderzoek MQTT Mosquito</t>
+  </si>
+  <si>
+    <t>Aansturen team</t>
+  </si>
+  <si>
+    <t>Logboek bijwerken.</t>
+  </si>
+  <si>
+    <t>Herverdelen taken.</t>
+  </si>
+  <si>
+    <t>Vergadering over server met ander team.</t>
+  </si>
+  <si>
+    <t>Afstemming netwerk gedeelte van proftaak met het ander team.</t>
+  </si>
+  <si>
+    <t>Week 9</t>
   </si>
 </sst>
 </file>
@@ -577,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78840537-239C-47B0-A4CC-46A5360523B1}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="A1:F3"/>
+    <sheetView tabSelected="1" topLeftCell="N27" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,26 +838,26 @@
         <v>7</v>
       </c>
       <c r="B7" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="9">
-        <v>0</v>
+        <v>16.25</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="10">
         <f xml:space="preserve"> D7 - B7 - F7</f>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>5</v>
@@ -850,26 +884,26 @@
         <v>8</v>
       </c>
       <c r="B8" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="10">
         <f xml:space="preserve"> D8 - B8 - F8</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>5</v>
@@ -896,26 +930,26 @@
         <v>9</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="10">
         <f xml:space="preserve"> D9- B9 - F9</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>5</v>
@@ -939,26 +973,26 @@
         <v>10</v>
       </c>
       <c r="B10" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="10">
         <f xml:space="preserve"> D10 - B10- F10</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>5</v>
@@ -973,26 +1007,26 @@
         <v>11</v>
       </c>
       <c r="B11" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="10">
         <f t="shared" ref="H11:H19" si="0" xml:space="preserve"> D11 - B11 - F11</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>5</v>
@@ -1022,26 +1056,26 @@
         <v>12</v>
       </c>
       <c r="B12" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f xml:space="preserve"> D12 - B12 - F12</f>
+        <v>5.5</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>5</v>
@@ -1068,26 +1102,26 @@
         <v>13</v>
       </c>
       <c r="B13" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>5</v>
@@ -1114,26 +1148,26 @@
         <v>14</v>
       </c>
       <c r="B14" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>5</v>
@@ -1198,7 +1232,7 @@
         <v>0.4201388888888889</v>
       </c>
       <c r="S15" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
@@ -1278,7 +1312,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="P17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q17" s="11">
         <v>0.4513888888888889</v>
@@ -1287,7 +1321,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="S17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
@@ -1324,7 +1358,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="P18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q18" s="11">
         <v>0.45833333333333331</v>
@@ -1376,7 +1410,7 @@
         <v>0.5</v>
       </c>
       <c r="S19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
@@ -1413,7 +1447,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="P20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q20" s="11">
         <v>0.5</v>
@@ -1456,7 +1490,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="P21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q21" s="11">
         <v>0.52083333333333337</v>
@@ -1499,7 +1533,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="P22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q22" s="11">
         <v>0.54166666666666663</v>
@@ -1514,28 +1548,28 @@
       </c>
       <c r="B23" s="5">
         <f>B4 + B5 + B6 + B7 + B8 + B9 + B11 + B12 + B13 + B14 + B15 + B16 + B17 + B18 + B19 + B20 + B21 + B22</f>
-        <v>17.5</v>
+        <v>80.5</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="6">
         <f>D4 + D5 + D6 + D7 + D8 + D9 + D10 + D11 + D12 + D13 + D14 + D15 + D16 + D17 + D18 + D19 + D20 + D21 + D22</f>
-        <v>31.515000000000001</v>
+        <v>152.76499999999999</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="5">
         <f>F4 + F5 + F6 + F7 + F8 + F9 + F10 + F11 + F12 + F13 + F14+ F15 + F16 + F17 + F18 + F19 + F20 + F21 + F22</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="7">
         <f xml:space="preserve"> H4 + H5 + H6 + H7 + H8 + H9 + H10 + H11 + H12 + H13 + H14 + H15 + H16 + H17 + H18 + H19 + H20 + H21 + H22</f>
-        <v>13.015000000000001</v>
+        <v>58.265000000000001</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>5</v>
@@ -1545,7 +1579,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="P23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q23" s="11">
         <v>0.625</v>
@@ -1569,13 +1603,16 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="P24" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="Q24" s="11">
         <v>0.66666666666666663</v>
       </c>
       <c r="R24" s="11">
         <v>0.67013888888888884</v>
+      </c>
+      <c r="S24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -1638,7 +1675,232 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M28" s="1"/>
       <c r="O28" t="s">
+        <v>43</v>
+      </c>
+      <c r="P28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>24</v>
+      </c>
+      <c r="R28" t="s">
+        <v>25</v>
+      </c>
+      <c r="S28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q29" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="R29" s="11">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q30" s="11">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="R30" s="11">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
         <v>45</v>
+      </c>
+      <c r="Q31" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="R31" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q32" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="R32" s="11">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="33" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q33" s="11">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="R33" s="11">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="34" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P34" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q34" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="R34" s="11">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="35" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P35" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q35" s="11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R35" s="11">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="S35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>48</v>
+      </c>
+      <c r="P37" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>24</v>
+      </c>
+      <c r="R37" t="s">
+        <v>25</v>
+      </c>
+      <c r="S37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q38" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="R38" s="11">
+        <v>0.40277777777777773</v>
+      </c>
+    </row>
+    <row r="39" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="11">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="R39" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="S39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q40" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="R40" s="11">
+        <v>0.43055555555555558</v>
+      </c>
+    </row>
+    <row r="41" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q41" s="11">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="R41" s="11">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="S41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P42" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q42" s="11">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="R42" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P43" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q43" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="R43" s="11">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="44" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P44" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q44" s="11">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="R44" s="11">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="46" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O46" t="s">
+        <v>56</v>
+      </c>
+      <c r="P46" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>24</v>
+      </c>
+      <c r="R46" t="s">
+        <v>25</v>
+      </c>
+      <c r="S46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="P47" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q47" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="R47" s="11">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="48" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="Q48" s="11">
+        <v>0.39583333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>